<commit_message>
[Modify] Pump : Static Method to Instance Method
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="pump_config_1" sheetId="1" r:id="rId1"/>
+    <sheet name="PumpConfig1" sheetId="1" r:id="rId1"/>
     <sheet name="compressor_config_1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>pipe_loss</t>
   </si>
@@ -89,6 +89,126 @@
   </si>
   <si>
     <t>premium_eff_motor</t>
+  </si>
+  <si>
+    <t>suction_pressure</t>
+  </si>
+  <si>
+    <t>discharge_pressure</t>
+  </si>
+  <si>
+    <t>cv_opening</t>
+  </si>
+  <si>
+    <t>downstream_pressure</t>
+  </si>
+  <si>
+    <t>motor_power</t>
+  </si>
+  <si>
+    <t>recirculation_flow</t>
+  </si>
+  <si>
+    <t>power_factor</t>
+  </si>
+  <si>
+    <t>run_status</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>motor_amp</t>
+  </si>
+  <si>
+    <t>flowrate_percent</t>
+  </si>
+  <si>
+    <t>differential_pressure</t>
+  </si>
+  <si>
+    <t>actual_cv</t>
+  </si>
+  <si>
+    <t>calculated_cv_drop</t>
+  </si>
+  <si>
+    <t>measured_cv_drop</t>
+  </si>
+  <si>
+    <t>cv_pressure_drop</t>
+  </si>
+  <si>
+    <t>inherent_piping_loss</t>
+  </si>
+  <si>
+    <t>required_differential_pressure</t>
+  </si>
+  <si>
+    <t>required_speed_variation</t>
+  </si>
+  <si>
+    <t>base_hydraulic_power</t>
+  </si>
+  <si>
+    <t>old_pump_efficiency</t>
+  </si>
+  <si>
+    <t>old_motor_efficiency</t>
+  </si>
+  <si>
+    <t>base_motor_power</t>
+  </si>
+  <si>
+    <t>selected_measure</t>
+  </si>
+  <si>
+    <t>selected_speed_variation</t>
+  </si>
+  <si>
+    <t>new_pump_efficiency</t>
+  </si>
+  <si>
+    <t>new_motor_efficiency</t>
+  </si>
+  <si>
+    <t>base_case_energy_consumption</t>
+  </si>
+  <si>
+    <t>proposed_case_energy_consumption</t>
+  </si>
+  <si>
+    <t>annual_energy_saving</t>
+  </si>
+  <si>
+    <t>base_case_emission</t>
+  </si>
+  <si>
+    <t>proposed_case_emission</t>
+  </si>
+  <si>
+    <t>annual_energy_savings</t>
+  </si>
+  <si>
+    <t>ghg_reduction</t>
+  </si>
+  <si>
+    <t>ghg_reduction_percent</t>
+  </si>
+  <si>
+    <t>mandatory_columns</t>
+  </si>
+  <si>
+    <t>computed_columns</t>
+  </si>
+  <si>
+    <t>optional_columns</t>
+  </si>
+  <si>
+    <t>energy_columns</t>
+  </si>
+  <si>
+    <t>emission_columns</t>
   </si>
 </sst>
 </file>
@@ -96,9 +216,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +228,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -199,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -211,10 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,20 +625,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -519,8 +653,23 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="G1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,8 +677,23 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -539,8 +703,23 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -548,8 +727,23 @@
         <v>0.01</v>
       </c>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -559,8 +753,20 @@
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -568,8 +774,20 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -577,8 +795,17 @@
         <v>0.7</v>
       </c>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -586,8 +813,17 @@
         <v>0.05</v>
       </c>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -597,8 +833,14 @@
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -606,13 +848,19 @@
         <v>0.75</v>
       </c>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
@@ -622,8 +870,11 @@
       <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -631,8 +882,11 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
@@ -642,8 +896,11 @@
       <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
@@ -652,7 +909,7 @@
       </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
@@ -661,7 +918,7 @@
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
@@ -670,7 +927,7 @@
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -679,7 +936,7 @@
       </c>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>22</v>
       </c>
@@ -702,9 +959,9 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
[Add] Economic & Emission Calculation
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>pipe_loss</t>
   </si>
@@ -70,9 +70,6 @@
     <t>USD/kW</t>
   </si>
   <si>
-    <t>impeller_replacement_cost</t>
-  </si>
-  <si>
     <t>motor_cost</t>
   </si>
   <si>
@@ -209,16 +206,57 @@
   </si>
   <si>
     <t>emission_columns</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>vsd_capex</t>
+  </si>
+  <si>
+    <t>vfd_capex</t>
+  </si>
+  <si>
+    <t>vsd_opex</t>
+  </si>
+  <si>
+    <t>vfd_opex</t>
+  </si>
+  <si>
+    <t>electricity_price</t>
+  </si>
+  <si>
+    <t>USD/MWh</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
+  </si>
+  <si>
+    <t>project_life</t>
+  </si>
+  <si>
+    <t>inflation_rate</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>impeller_capex</t>
+  </si>
+  <si>
+    <t>impeller_opex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +279,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4FC1FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -273,79 +317,32 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -625,16 +622,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.140625" customWidth="1"/>
@@ -653,20 +651,20 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -678,19 +676,19 @@
       </c>
       <c r="C2" s="1"/>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -704,19 +702,19 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -731,16 +729,16 @@
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -754,16 +752,16 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -775,16 +773,16 @@
       </c>
       <c r="C6" s="1"/>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -796,13 +794,13 @@
       </c>
       <c r="C7" s="1"/>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -814,13 +812,13 @@
       </c>
       <c r="C8" s="1"/>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -834,10 +832,10 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -849,101 +847,193 @@
       </c>
       <c r="C10" s="1"/>
       <c r="K10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="K13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="K11" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1235000</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="9">
+        <v>5000000</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="11">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="12">
+        <v>500</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="K19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6">
-        <v>500</v>
-      </c>
-      <c r="C12" s="9" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="9">
+        <v>200000</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>300</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="K13" t="s">
+      <c r="K22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="8">
-        <v>300</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="B23" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="10">
-        <v>0.17</v>
-      </c>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="B24" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="10">
-        <v>0.34</v>
-      </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="B25" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="11">
-        <v>0.95</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="B26" s="13">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="11">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="13">
+      <c r="B27" s="13">
         <v>0.97</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,6 +1043,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
[Add] Report in Tasklist, Emission Factor
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PumpConfig1" sheetId="1" r:id="rId1"/>
-    <sheet name="compressor_config_1" sheetId="2" r:id="rId2"/>
+    <sheet name="EmissionFactor" sheetId="4" r:id="rId2"/>
+    <sheet name="compressor_config_1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>pipe_loss</t>
   </si>
@@ -88,126 +89,6 @@
     <t>premium_eff_motor</t>
   </si>
   <si>
-    <t>suction_pressure</t>
-  </si>
-  <si>
-    <t>discharge_pressure</t>
-  </si>
-  <si>
-    <t>cv_opening</t>
-  </si>
-  <si>
-    <t>downstream_pressure</t>
-  </si>
-  <si>
-    <t>motor_power</t>
-  </si>
-  <si>
-    <t>recirculation_flow</t>
-  </si>
-  <si>
-    <t>power_factor</t>
-  </si>
-  <si>
-    <t>run_status</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
-  <si>
-    <t>motor_amp</t>
-  </si>
-  <si>
-    <t>flowrate_percent</t>
-  </si>
-  <si>
-    <t>differential_pressure</t>
-  </si>
-  <si>
-    <t>actual_cv</t>
-  </si>
-  <si>
-    <t>calculated_cv_drop</t>
-  </si>
-  <si>
-    <t>measured_cv_drop</t>
-  </si>
-  <si>
-    <t>cv_pressure_drop</t>
-  </si>
-  <si>
-    <t>inherent_piping_loss</t>
-  </si>
-  <si>
-    <t>required_differential_pressure</t>
-  </si>
-  <si>
-    <t>required_speed_variation</t>
-  </si>
-  <si>
-    <t>base_hydraulic_power</t>
-  </si>
-  <si>
-    <t>old_pump_efficiency</t>
-  </si>
-  <si>
-    <t>old_motor_efficiency</t>
-  </si>
-  <si>
-    <t>base_motor_power</t>
-  </si>
-  <si>
-    <t>selected_measure</t>
-  </si>
-  <si>
-    <t>selected_speed_variation</t>
-  </si>
-  <si>
-    <t>new_pump_efficiency</t>
-  </si>
-  <si>
-    <t>new_motor_efficiency</t>
-  </si>
-  <si>
-    <t>base_case_energy_consumption</t>
-  </si>
-  <si>
-    <t>proposed_case_energy_consumption</t>
-  </si>
-  <si>
-    <t>annual_energy_saving</t>
-  </si>
-  <si>
-    <t>base_case_emission</t>
-  </si>
-  <si>
-    <t>proposed_case_emission</t>
-  </si>
-  <si>
-    <t>annual_energy_savings</t>
-  </si>
-  <si>
-    <t>ghg_reduction</t>
-  </si>
-  <si>
-    <t>ghg_reduction_percent</t>
-  </si>
-  <si>
-    <t>mandatory_columns</t>
-  </si>
-  <si>
-    <t>computed_columns</t>
-  </si>
-  <si>
-    <t>optional_columns</t>
-  </si>
-  <si>
-    <t>energy_columns</t>
-  </si>
-  <si>
-    <t>emission_columns</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -245,18 +126,55 @@
   </si>
   <si>
     <t>impeller_opex</t>
+  </si>
+  <si>
+    <t>DAS</t>
+  </si>
+  <si>
+    <t>ZIRKU</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>NASR</t>
+  </si>
+  <si>
+    <t>LZ</t>
+  </si>
+  <si>
+    <t>UZ</t>
+  </si>
+  <si>
+    <t>SARB</t>
+  </si>
+  <si>
+    <t>UL</t>
+  </si>
+  <si>
+    <t>UAD</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>ABK</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,17 +191,24 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF4FC1FF"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -318,31 +243,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -623,10 +553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,14 +564,10 @@
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
-    <col min="9" max="9" width="36.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -651,23 +577,8 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,23 +586,8 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -701,23 +597,8 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -725,23 +606,8 @@
         <v>0.01</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -751,20 +617,8 @@
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -772,20 +626,8 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -793,17 +635,8 @@
         <v>0.7</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -811,34 +644,19 @@
         <v>0.05</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="5">
-        <v>0.45</v>
+        <v>1.081</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -846,137 +664,121 @@
         <v>0.75</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="K10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2">
         <v>0.09</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5">
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="8">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6">
         <v>0.02</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="K13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="9">
+        <v>23</v>
+      </c>
+      <c r="B14" s="7">
         <v>1235000</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="9">
+        <v>24</v>
+      </c>
+      <c r="B15" s="7">
         <v>5000000</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="10">
+        <v>25</v>
+      </c>
+      <c r="B16" s="8">
         <v>0.04</v>
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="10">
+        <v>26</v>
+      </c>
+      <c r="B17" s="8">
         <v>0.02</v>
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="11">
+        <v>27</v>
+      </c>
+      <c r="B18" s="9">
         <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="10">
         <v>500</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="K19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="9">
+        <v>33</v>
+      </c>
+      <c r="B20" s="7">
         <v>200000</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="7"/>
-      <c r="K20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="9">
+        <v>34</v>
+      </c>
+      <c r="B21" s="7">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -986,11 +788,8 @@
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -999,7 +798,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -1008,29 +807,29 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="11">
         <v>0.95</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="11">
         <v>0.95599999999999996</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="11">
         <v>0.97</v>
       </c>
       <c r="C27" s="1"/>
@@ -1043,11 +842,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1.081</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2.286</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K20" sqref="J20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Major Refactoring all the column names with seperate definitions class
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6DCAC-0D86-4DB5-9F91-1E70673A646E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-21156" yWindow="2928" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PumpConfig1" sheetId="1" r:id="rId1"/>
-    <sheet name="EmissionFactor" sheetId="4" r:id="rId2"/>
+    <sheet name="Emission Factor" sheetId="4" r:id="rId2"/>
     <sheet name="compressor_config_1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -23,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
-    <t>pipe_loss</t>
-  </si>
-  <si>
-    <t>min_cv_loss</t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
@@ -41,93 +47,21 @@
     <t>unit</t>
   </si>
   <si>
-    <t>min_cv_opening</t>
-  </si>
-  <si>
-    <t>discharge_flowrate</t>
-  </si>
-  <si>
-    <t>min_working_percent</t>
-  </si>
-  <si>
-    <t>min_speed</t>
-  </si>
-  <si>
-    <t>bin_percent</t>
-  </si>
-  <si>
-    <t>emission_factor</t>
-  </si>
-  <si>
     <t>tCO2/MWh</t>
   </si>
   <si>
-    <t>pump_efficiency</t>
-  </si>
-  <si>
-    <t>pump_cost</t>
-  </si>
-  <si>
     <t>USD/kW</t>
   </si>
   <si>
-    <t>motor_cost</t>
-  </si>
-  <si>
-    <t>high_eff_escalation_factor</t>
-  </si>
-  <si>
-    <t>premium_eff_escalation_factor</t>
-  </si>
-  <si>
-    <t>std_eff_motor</t>
-  </si>
-  <si>
-    <t>high_eff_motor</t>
-  </si>
-  <si>
-    <t>premium_eff_motor</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
-    <t>vsd_capex</t>
-  </si>
-  <si>
-    <t>vfd_capex</t>
-  </si>
-  <si>
-    <t>vsd_opex</t>
-  </si>
-  <si>
-    <t>vfd_opex</t>
-  </si>
-  <si>
-    <t>electricity_price</t>
-  </si>
-  <si>
     <t>USD/MWh</t>
   </si>
   <si>
-    <t>discount_rate</t>
-  </si>
-  <si>
-    <t>project_life</t>
-  </si>
-  <si>
-    <t>inflation_rate</t>
-  </si>
-  <si>
     <t>years</t>
   </si>
   <si>
-    <t>impeller_capex</t>
-  </si>
-  <si>
-    <t>impeller_opex</t>
-  </si>
-  <si>
     <t>DAS</t>
   </si>
   <si>
@@ -162,12 +96,90 @@
   </si>
   <si>
     <t>site</t>
+  </si>
+  <si>
+    <t>Piping Loss</t>
+  </si>
+  <si>
+    <t>Min CV Loss</t>
+  </si>
+  <si>
+    <t>Min CV Opening</t>
+  </si>
+  <si>
+    <t>Discharge Flowrate</t>
+  </si>
+  <si>
+    <t>Min Working Percent</t>
+  </si>
+  <si>
+    <t>Min Speed</t>
+  </si>
+  <si>
+    <t>Bin Percent</t>
+  </si>
+  <si>
+    <t>Emission Factor</t>
+  </si>
+  <si>
+    <t>Pump Efficiency</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>Project Life</t>
+  </si>
+  <si>
+    <t>Inflation Rate</t>
+  </si>
+  <si>
+    <t>VSD Capex</t>
+  </si>
+  <si>
+    <t>VSD Opex</t>
+  </si>
+  <si>
+    <t>Electricity Price</t>
+  </si>
+  <si>
+    <t>Pump Cost</t>
+  </si>
+  <si>
+    <t>Impeller Capex</t>
+  </si>
+  <si>
+    <t>Impeller Opex</t>
+  </si>
+  <si>
+    <t>Motor Cost</t>
+  </si>
+  <si>
+    <t>High Eff Escalation Factor</t>
+  </si>
+  <si>
+    <t>Premium Eff Escalation Factor</t>
+  </si>
+  <si>
+    <t>Std Eff Motor</t>
+  </si>
+  <si>
+    <t>High Eff Motor</t>
+  </si>
+  <si>
+    <t>Premium Eff Motor</t>
+  </si>
+  <si>
+    <t>VFD Capex</t>
+  </si>
+  <si>
+    <t>VFD Opex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -248,32 +260,30 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -550,285 +560,285 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2">
         <v>0.2</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>0.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>0.01</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="2">
         <v>0.7</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B8" s="2">
         <v>0.05</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="4">
         <v>1.081</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>0.75</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="2">
         <v>0.09</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4">
         <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>0.02</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="7">
+        <v>33</v>
+      </c>
+      <c r="B14" s="6">
         <v>3000000</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="7">
+        <v>45</v>
+      </c>
+      <c r="B15" s="6">
         <v>7000000</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="8">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7">
         <v>0.04</v>
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="8">
+        <v>46</v>
+      </c>
+      <c r="B17" s="7">
         <v>0.02</v>
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="9">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1">
         <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="10">
+        <v>36</v>
+      </c>
+      <c r="B19" s="8">
         <v>500</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="7">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6">
         <v>100000</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="7">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1">
         <v>300</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2">
         <v>0.17</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2">
         <v>0.34</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="11">
+        <v>42</v>
+      </c>
+      <c r="B25" s="9">
         <v>0.95</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="11">
+        <v>43</v>
+      </c>
+      <c r="B26" s="9">
         <v>0.95599999999999996</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="11">
+        <v>44</v>
+      </c>
+      <c r="B27" s="9">
         <v>0.97</v>
       </c>
       <c r="C27" s="1"/>
@@ -840,111 +850,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="13">
+      <c r="B4" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="13">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="13">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="13">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="13">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="14">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="12">
         <v>0.66400000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="14">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="12">
         <v>1.081</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="14">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="12">
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="14">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12">
         <v>2.286</v>
       </c>
     </row>
@@ -954,7 +964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -962,17 +972,17 @@
       <selection activeCell="K20" sqref="J20:K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>